<commit_message>
maf excel help tabs deleted
</commit_message>
<xml_diff>
--- a/assets/files/submission/metabobank/MetaboBank_maf_MS.xlsx
+++ b/assets/files/submission/metabobank/MetaboBank_maf_MS.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8952"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17436" windowHeight="11124"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="12" r:id="rId1"/>
     <sheet name="MB_MAF" sheetId="16" r:id="rId2"/>
-    <sheet name="MB_MAF HELP" sheetId="17" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>database_identifier</t>
   </si>
@@ -74,40 +73,6 @@
     <t>search_engine_score</t>
   </si>
   <si>
-    <t># From here, enter the sample names and measured values.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Metabolite information should include all metabolites/unknowns/features identified within the study. You should complete the table with as much information as possible (note you can leave smiles/InChI empty as these can be auto completed from metabolite names or database identifiers during curation). Sample names should be included in the columns to the right of the table, in each column sample values per metabolite should be included.
-The metabolite table file (MTBKSxxx.maf.txt) should be referenced in the metabolite assignment file column of each assay (SDRF).each.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[M+H]+</t>
-  </si>
-  <si>
-    <t>C4H9N3O2</t>
-  </si>
-  <si>
-    <t>CN(CC(O)=O)C(N)=N</t>
-  </si>
-  <si>
-    <t>InChI=1S/C4H9N3O2/c1-7(4(5)6)2-3(8)9/h2H2,1H3,(H3,5,6)(H,8,9)</t>
-  </si>
-  <si>
-    <t>creatine</t>
-  </si>
-  <si>
-    <t>132,0870 l 90,0617 l 87,0618</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t># MAF (Metabolite Assignment File)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve"># TO MAKE A SUBMISSION: </t>
   </si>
   <si>
@@ -144,88 +109,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t># See HELP tabs to view definition, or see https://www.ddbj.nig.ac.jp/metabobank</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>peak_identifier</t>
   </si>
   <si>
     <t># From here, enter sample names and measured values.</t>
   </si>
   <si>
-    <t>Database identifier for metabolite. ChEBI ID is recommended. This is optional field.</t>
-  </si>
-  <si>
-    <t>Chemical formula of metabolite. This is optional field.</t>
-  </si>
-  <si>
-    <t>SMILES of metabolite. This is optional field.</t>
-  </si>
-  <si>
-    <t>INCHI key of metabolite.  This is optional field.</t>
-  </si>
-  <si>
-    <t>Identified metabolite name.</t>
-  </si>
-  <si>
-    <t>The mass to charge (m/z) ratio.</t>
-  </si>
-  <si>
-    <t>Fragmentation</t>
-  </si>
-  <si>
-    <t>Chemical modifications.</t>
-  </si>
-  <si>
-    <t>Retention time</t>
-  </si>
-  <si>
-    <t>The NCBI taxonomy id for the organism from which the metabolite was obtained. https://www.ncbi.nlm.nih.gov/Taxonomy/Browser/wwwtax.cgi</t>
-  </si>
-  <si>
-    <t>Species name of the NCBI taxonomy.</t>
-  </si>
-  <si>
-    <t>The database name used for metabolite identification.</t>
-  </si>
-  <si>
-    <t>The database version used for metabolite identification.</t>
-  </si>
-  <si>
-    <t>Reliability. Identification confidence of the metabolite. See https://www.ebi.ac.uk/metabolights/guides/Quick_start_Guide/Study%20Overview</t>
-  </si>
-  <si>
-    <t>Search engine</t>
-  </si>
-  <si>
-    <t>Search engine score</t>
-  </si>
-  <si>
-    <t>CHEBI:16919</t>
-  </si>
-  <si>
-    <t>9606</t>
-  </si>
-  <si>
-    <t>Homo sapiens</t>
-  </si>
-  <si>
-    <t>CHEBI</t>
-  </si>
-  <si>
-    <t>Field</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Readme</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Example</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t># MAF (Metabolite Assignment File) - MS</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -242,11 +131,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Class of metabolite</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>flavonoids</t>
+    <t># To view definition, see https://www.ddbj.nig.ac.jp/metabobank/datafile-e.html</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -254,11 +139,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,13 +167,6 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +202,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -338,27 +215,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="12">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="通貨" xfId="12" builtinId="7"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="3" builtinId="9" hidden="1"/>
@@ -682,9 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="A15:B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -694,95 +560,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>64</v>
+      <c r="A1" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>34</v>
+      <c r="A4" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>27</v>
+      <c r="A5" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>28</v>
+      <c r="A6" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>29</v>
+      <c r="A7" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>30</v>
+      <c r="A8" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6">
+        <v>44851</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6">
+        <v>44509</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="6">
+        <v>44645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="9">
-        <v>44645</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="9">
-        <v>44509</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="9">
-        <v>44645</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <v>44763</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
+      <c r="B16" s="6"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
+      <c r="B17" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -847,14 +713,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>63</v>
+      <c r="A1" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="3"/>
       <c r="T2" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -874,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>5</v>
@@ -913,248 +779,7 @@
         <v>16</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V23"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="67.33203125" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="67.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="11">
-        <v>132.07650000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0.85</v>
-      </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>